<commit_message>
A few changes improving repair list page and first tries with filter with extra words below input field.
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="299">
   <si>
     <t>hashId</t>
   </si>
@@ -935,6 +935,18 @@
   </si>
   <si>
     <t>"2017-04-08T23:54:58.000Z"</t>
+  </si>
+  <si>
+    <t>Dodać obsługę w backendzie zapisywania maszyny i obszaru</t>
+  </si>
+  <si>
+    <t>Dodać walidację pól które mają mieć konkretne wartośći - np. maszyna i obszar</t>
+  </si>
+  <si>
+    <t>Dodać walidację formularza dodawania napraw</t>
+  </si>
+  <si>
+    <t>Dodać obsługę przycisku w dół i górę odnośnie zaznaczania słowa do wybrania - jak w google'u</t>
   </si>
 </sst>
 </file>
@@ -2715,8 +2727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="A125" sqref="A125"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="A129" sqref="A129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3322,7 +3334,7 @@
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="18" t="s">
+      <c r="A116" s="16" t="s">
         <v>275</v>
       </c>
       <c r="D116" t="s">
@@ -3418,6 +3430,26 @@
       </c>
       <c r="F124" t="s">
         <v>236</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="129" spans="4:6" ht="42.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
First tests of adding multiline references and check them with regular expressions
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="307">
   <si>
     <t>hashId</t>
   </si>
@@ -948,17 +948,49 @@
   <si>
     <t>Dodać obsługę przycisku w dół i górę odnośnie zaznaczania słowa do wybrania - jak w google'u</t>
   </si>
+  <si>
+    <t>10.04.2017</t>
+  </si>
+  <si>
+    <t>M20V00004</t>
+  </si>
+  <si>
+    <t>M20V00005</t>
+  </si>
+  <si>
+    <t>M20V00007</t>
+  </si>
+  <si>
+    <t>M20V00009</t>
+  </si>
+  <si>
+    <t>M20V0000</t>
+  </si>
+  <si>
+    <t>M20a00008</t>
+  </si>
+  <si>
+    <t>M20Vcc1010</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1235,10 +1267,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1255,31 +1287,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1287,6 +1312,12 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1979,8 +2010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2549,7 +2580,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="36" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -2558,7 +2589,7 @@
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
+      <c r="A3" s="36"/>
       <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
@@ -2567,7 +2598,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
@@ -2576,7 +2607,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
@@ -2585,7 +2616,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="9" t="s">
         <v>19</v>
       </c>
@@ -2594,7 +2625,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="9" t="s">
         <v>18</v>
       </c>
@@ -2603,7 +2634,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
@@ -2612,7 +2643,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="29"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="9" t="s">
         <v>7</v>
       </c>
@@ -2621,7 +2652,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="9" t="s">
         <v>11</v>
       </c>
@@ -2631,7 +2662,7 @@
       <c r="D10" s="14"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="29"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="6" t="s">
         <v>12</v>
       </c>
@@ -2641,7 +2672,7 @@
       <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
@@ -2654,7 +2685,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="29"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
@@ -2665,7 +2696,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
@@ -2678,7 +2709,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="29"/>
+      <c r="A15" s="36"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
@@ -2725,10 +2756,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F144"/>
+  <dimension ref="A1:F151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="A124" sqref="A124"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="D145" sqref="D145:D151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3216,8 +3247,11 @@
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="30" t="s">
+      <c r="A105" s="26" t="s">
         <v>261</v>
+      </c>
+      <c r="B105" t="s">
+        <v>299</v>
       </c>
       <c r="D105" t="s">
         <v>237</v>
@@ -3249,8 +3283,11 @@
       </c>
     </row>
     <row r="108" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="31" t="s">
+      <c r="A108" s="35" t="s">
         <v>264</v>
+      </c>
+      <c r="B108" t="s">
+        <v>299</v>
       </c>
       <c r="D108" t="s">
         <v>240</v>
@@ -3260,8 +3297,11 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="30" t="s">
+      <c r="A109" s="26" t="s">
         <v>265</v>
+      </c>
+      <c r="B109" t="s">
+        <v>299</v>
       </c>
       <c r="D109" t="s">
         <v>241</v>
@@ -3271,8 +3311,11 @@
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="30" t="s">
+      <c r="A110" s="26" t="s">
         <v>266</v>
+      </c>
+      <c r="B110" t="s">
+        <v>299</v>
       </c>
       <c r="D110" t="s">
         <v>242</v>
@@ -3282,8 +3325,11 @@
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="30" t="s">
+      <c r="A111" s="26" t="s">
         <v>267</v>
+      </c>
+      <c r="B111" t="s">
+        <v>299</v>
       </c>
       <c r="D111" t="s">
         <v>243</v>
@@ -3301,7 +3347,7 @@
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="33" t="s">
+      <c r="A113" s="30" t="s">
         <v>272</v>
       </c>
       <c r="D113" t="s">
@@ -3312,7 +3358,7 @@
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="32" t="s">
+      <c r="A114" s="29" t="s">
         <v>273</v>
       </c>
       <c r="D114" t="s">
@@ -3452,53 +3498,53 @@
         <v>298</v>
       </c>
     </row>
-    <row r="129" spans="4:6" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="D129" s="34" t="s">
+    <row r="129" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D129" s="31" t="s">
         <v>284</v>
       </c>
-      <c r="E129" s="34" t="s">
+      <c r="E129" s="31" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="130" spans="4:6" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="D130" s="34" t="s">
+    <row r="130" spans="4:6" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="D130" s="31" t="s">
         <v>285</v>
       </c>
-      <c r="E130" s="34" t="s">
+      <c r="E130" s="31" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="131" spans="4:6" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="D131" s="34" t="s">
+    <row r="131" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="D131" s="31" t="s">
         <v>286</v>
       </c>
-      <c r="E131" s="34" t="s">
+      <c r="E131" s="31" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="132" spans="4:6" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="D132" s="34" t="s">
+    <row r="132" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D132" s="31" t="s">
         <v>287</v>
       </c>
-      <c r="E132" s="34" t="s">
+      <c r="E132" s="31" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="133" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D133" s="35">
+      <c r="D133" s="32">
         <v>42827</v>
       </c>
-      <c r="E133" s="35">
+      <c r="E133" s="32">
         <v>42827</v>
       </c>
     </row>
-    <row r="134" spans="4:6" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="E134" s="34" t="s">
+    <row r="134" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E134" s="31" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="135" spans="4:6" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="E135" s="34" t="s">
+    <row r="135" spans="4:6" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="E135" s="31" t="s">
         <v>288</v>
       </c>
     </row>
@@ -3506,90 +3552,125 @@
       <c r="D136" t="s">
         <v>291</v>
       </c>
-      <c r="E136" s="34" t="s">
+      <c r="E136" s="31" t="s">
         <v>292</v>
       </c>
       <c r="F136" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="137" spans="4:6" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="D137" s="34" t="s">
+    <row r="137" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D137" s="31" t="s">
         <v>284</v>
       </c>
-      <c r="E137" s="36" t="s">
+      <c r="E137" s="33" t="s">
         <v>284</v>
       </c>
-      <c r="F137" s="34" t="s">
+      <c r="F137" s="31" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="138" spans="4:6" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="D138" s="34" t="s">
+    <row r="138" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="D138" s="31" t="s">
         <v>289</v>
       </c>
-      <c r="E138" s="36" t="s">
+      <c r="E138" s="33" t="s">
         <v>289</v>
       </c>
-      <c r="F138" s="34" t="s">
+      <c r="F138" s="31" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="139" spans="4:6" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="D139" s="34" t="s">
+    <row r="139" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="D139" s="31" t="s">
         <v>286</v>
       </c>
-      <c r="E139" s="36" t="s">
+      <c r="E139" s="33" t="s">
         <v>286</v>
       </c>
-      <c r="F139" s="34" t="s">
+      <c r="F139" s="31" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="140" spans="4:6" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="D140" s="34" t="s">
+    <row r="140" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="D140" s="31" t="s">
         <v>290</v>
       </c>
-      <c r="E140" s="36" t="s">
+      <c r="E140" s="33" t="s">
         <v>290</v>
       </c>
-      <c r="F140" s="34" t="s">
+      <c r="F140" s="31" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="141" spans="4:6" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="D141" s="34" t="s">
+    <row r="141" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D141" s="31" t="s">
         <v>287</v>
       </c>
-      <c r="E141" s="36" t="s">
+      <c r="E141" s="33" t="s">
         <v>287</v>
       </c>
-      <c r="F141" s="34" t="s">
+      <c r="F141" s="31" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="142" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D142" s="34" t="s">
+      <c r="D142" s="31" t="s">
         <v>258</v>
       </c>
-      <c r="E142" s="37">
+      <c r="E142" s="34">
         <v>42834</v>
       </c>
-      <c r="F142" s="35">
+      <c r="F142" s="32">
         <v>42834</v>
       </c>
     </row>
-    <row r="143" spans="4:6" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="E143" s="34" t="s">
+    <row r="143" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E143" s="31" t="s">
         <v>258</v>
       </c>
-      <c r="F143" s="34" t="s">
+      <c r="F143" s="31" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="144" spans="4:6" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="F144" s="34" t="s">
+    <row r="144" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="F144" s="31" t="s">
         <v>294</v>
+      </c>
+    </row>
+    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D145" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D146" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D147" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D148" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D149" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D150" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D151" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working new possibility of adding planty of references by textarea with reg exp check
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="319">
   <si>
     <t>hashId</t>
   </si>
@@ -972,12 +972,48 @@
   <si>
     <t>M20Vcc1010</t>
   </si>
+  <si>
+    <t>MS08</t>
+  </si>
+  <si>
+    <t>+ 5 znaków</t>
+  </si>
+  <si>
+    <t>MP4A</t>
+  </si>
+  <si>
+    <t>M2GA</t>
+  </si>
+  <si>
+    <t>M20VC</t>
+  </si>
+  <si>
+    <t>+ 4 znaki</t>
+  </si>
+  <si>
+    <t>M20V</t>
+  </si>
+  <si>
+    <t>M20M</t>
+  </si>
+  <si>
+    <t>M20G</t>
+  </si>
+  <si>
+    <t>M20VP</t>
+  </si>
+  <si>
+    <t>Dane do wyrażeń regularnych kontroli nowych referencji</t>
+  </si>
+  <si>
+    <t>M20V03443</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1067,6 +1103,13 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -1112,7 +1155,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1263,11 +1306,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1315,6 +1373,18 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -2580,7 +2650,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="40" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -2589,7 +2659,7 @@
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
+      <c r="A3" s="40"/>
       <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
@@ -2598,7 +2668,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
@@ -2607,7 +2677,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
@@ -2616,7 +2686,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="9" t="s">
         <v>19</v>
       </c>
@@ -2625,7 +2695,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="9" t="s">
         <v>18</v>
       </c>
@@ -2634,7 +2704,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
@@ -2643,7 +2713,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="36"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="9" t="s">
         <v>7</v>
       </c>
@@ -2652,7 +2722,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="36"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="9" t="s">
         <v>11</v>
       </c>
@@ -2662,7 +2732,7 @@
       <c r="D10" s="14"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="36"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="6" t="s">
         <v>12</v>
       </c>
@@ -2672,7 +2742,7 @@
       <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="36"/>
+      <c r="A12" s="40"/>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
@@ -2685,7 +2755,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="36"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
@@ -2696,7 +2766,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
@@ -2709,7 +2779,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="36"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
@@ -2744,22 +2814,98 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="36" t="s">
+        <v>307</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="38" t="s">
+        <v>309</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="38" t="s">
+        <v>310</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="38" t="s">
+        <v>313</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="38" t="s">
+        <v>315</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="38" t="s">
+        <v>316</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>312</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F151"/>
+  <dimension ref="A1:F152"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="D145" sqref="D145:D151"/>
+      <selection activeCell="D145" sqref="D145:D152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3671,6 +3817,11 @@
     <row r="151" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D151" t="s">
         <v>306</v>
+      </c>
+    </row>
+    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D152" t="s">
+        <v>318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New functionality of adding M20V references with one textarea - very flexible
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="331">
   <si>
     <t>hashId</t>
   </si>
@@ -1007,6 +1007,42 @@
   </si>
   <si>
     <t>M20V03443</t>
+  </si>
+  <si>
+    <t>!!! Dodać filtr na głownym oknie narzędzi - W naprawie, Po naprawie nieodebrane, Po naprawie odebrane, Dostępne - z kolorami</t>
+  </si>
+  <si>
+    <t>Dodać kolorwanie nagłówków w zależności od statusu narzędzia</t>
+  </si>
+  <si>
+    <t>Dodać ostatniego edytora zmian na narzędziu</t>
+  </si>
+  <si>
+    <t>- MP4A + 5 znaków</t>
+  </si>
+  <si>
+    <t>- MP40 + 5 znaków</t>
+  </si>
+  <si>
+    <t>- MK20V + 5 znaków</t>
+  </si>
+  <si>
+    <t>- M5KA + 5 znaków</t>
+  </si>
+  <si>
+    <t>- M5EA + 5 znaków</t>
+  </si>
+  <si>
+    <t>- N20V + 5 znaków</t>
+  </si>
+  <si>
+    <t>- M772 + 5 znaków</t>
+  </si>
+  <si>
+    <t>- M20V + 5 znaków</t>
+  </si>
+  <si>
+    <t>To pokrywa się z M20V + 5 znaków</t>
   </si>
 </sst>
 </file>
@@ -1325,7 +1361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1374,13 +1410,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1389,6 +1419,25 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2650,7 +2699,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="38" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -2659,7 +2708,7 @@
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
+      <c r="A3" s="38"/>
       <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
@@ -2668,7 +2717,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
@@ -2677,7 +2726,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
@@ -2686,7 +2735,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
+      <c r="A6" s="38"/>
       <c r="B6" s="9" t="s">
         <v>19</v>
       </c>
@@ -2695,7 +2744,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="9" t="s">
         <v>18</v>
       </c>
@@ -2704,7 +2753,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
+      <c r="A8" s="38"/>
       <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
@@ -2713,7 +2762,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="40"/>
+      <c r="A9" s="38"/>
       <c r="B9" s="9" t="s">
         <v>7</v>
       </c>
@@ -2722,7 +2771,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="9" t="s">
         <v>11</v>
       </c>
@@ -2732,7 +2781,7 @@
       <c r="D10" s="14"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="40"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="6" t="s">
         <v>12</v>
       </c>
@@ -2742,7 +2791,7 @@
       <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
+      <c r="A12" s="38"/>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
@@ -2755,7 +2804,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="40"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
@@ -2766,7 +2815,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
@@ -2779,7 +2828,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="40"/>
+      <c r="A15" s="38"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
@@ -2814,10 +2863,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2825,73 +2874,125 @@
     <col min="2" max="2" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="42" t="s">
         <v>307</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="36" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="43" t="s">
         <v>309</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="37" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="43" t="s">
         <v>310</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="37" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="38" t="s">
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="39" t="s">
         <v>311</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="40" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+      <c r="C5" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="43" t="s">
         <v>313</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="41" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="38" t="s">
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="43" t="s">
         <v>314</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="37" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="38" t="s">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="43" t="s">
         <v>315</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="37" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="38" t="s">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="39" t="s">
         <v>316</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="40" t="s">
         <v>312</v>
+      </c>
+      <c r="C9" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="44" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="44" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="44" t="s">
+        <v>322</v>
+      </c>
+      <c r="E13" s="18"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="44" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="44" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="44" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="44" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="44" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="44" t="s">
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -2902,10 +3003,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F152"/>
+  <dimension ref="A1:F157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="D145" sqref="D145:D152"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="A150" sqref="A150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3644,7 +3745,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="129" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D129" s="31" t="s">
         <v>284</v>
       </c>
@@ -3652,7 +3753,10 @@
         <v>284</v>
       </c>
     </row>
-    <row r="130" spans="4:6" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>319</v>
+      </c>
       <c r="D130" s="31" t="s">
         <v>285</v>
       </c>
@@ -3660,7 +3764,10 @@
         <v>285</v>
       </c>
     </row>
-    <row r="131" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>320</v>
+      </c>
       <c r="D131" s="31" t="s">
         <v>286</v>
       </c>
@@ -3668,7 +3775,10 @@
         <v>286</v>
       </c>
     </row>
-    <row r="132" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>321</v>
+      </c>
       <c r="D132" s="31" t="s">
         <v>287</v>
       </c>
@@ -3676,7 +3786,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="133" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D133" s="32">
         <v>42827</v>
       </c>
@@ -3684,17 +3794,17 @@
         <v>42827</v>
       </c>
     </row>
-    <row r="134" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E134" s="31" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="135" spans="4:6" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" ht="42.75" x14ac:dyDescent="0.25">
       <c r="E135" s="31" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="136" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D136" t="s">
         <v>291</v>
       </c>
@@ -3705,7 +3815,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="137" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D137" s="31" t="s">
         <v>284</v>
       </c>
@@ -3716,7 +3826,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="138" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="D138" s="31" t="s">
         <v>289</v>
       </c>
@@ -3727,7 +3837,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="139" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="D139" s="31" t="s">
         <v>286</v>
       </c>
@@ -3738,7 +3848,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="140" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="D140" s="31" t="s">
         <v>290</v>
       </c>
@@ -3749,7 +3859,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="141" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D141" s="31" t="s">
         <v>287</v>
       </c>
@@ -3760,7 +3870,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="142" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D142" s="31" t="s">
         <v>258</v>
       </c>
@@ -3771,7 +3881,7 @@
         <v>42834</v>
       </c>
     </row>
-    <row r="143" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E143" s="31" t="s">
         <v>258</v>
       </c>
@@ -3779,18 +3889,18 @@
         <v>258</v>
       </c>
     </row>
-    <row r="144" spans="4:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="F144" s="31" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="145" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D145" t="s">
+      <c r="D145" s="45" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="146" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D146" t="s">
+      <c r="D146" s="45" t="s">
         <v>301</v>
       </c>
     </row>
@@ -3800,17 +3910,17 @@
       </c>
     </row>
     <row r="148" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D148" t="s">
+      <c r="D148" s="45" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="149" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D149" t="s">
+      <c r="D149" s="17" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="150" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D150" t="s">
+      <c r="D150" s="45" t="s">
         <v>303</v>
       </c>
     </row>
@@ -3822,6 +3932,31 @@
     <row r="152" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D152" t="s">
         <v>318</v>
+      </c>
+    </row>
+    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D153" s="45" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D154" s="45" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="155" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D155" s="45" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D156" s="45" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="157" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D157" s="45" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish adding MASS* and M20V* references by textarea - all functionality is ready to test in production.
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="338">
   <si>
     <t>hashId</t>
   </si>
@@ -1044,17 +1044,46 @@
   <si>
     <t>To pokrywa się z M20V + 5 znaków</t>
   </si>
+  <si>
+    <t>MASS00001</t>
+  </si>
+  <si>
+    <t>MASS00221</t>
+  </si>
+  <si>
+    <t>MASS01374</t>
+  </si>
+  <si>
+    <t>MASS00384</t>
+  </si>
+  <si>
+    <t>M20V00001</t>
+  </si>
+  <si>
+    <t>MAD012345</t>
+  </si>
+  <si>
+    <t>MAAS00221</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1363,8 +1392,8 @@
   </cellStyleXfs>
   <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1381,24 +1410,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1407,37 +1436,37 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2699,7 +2728,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="45" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -2708,7 +2737,7 @@
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
+      <c r="A3" s="45"/>
       <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
@@ -2717,7 +2746,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
@@ -2726,7 +2755,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
+      <c r="A5" s="45"/>
       <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
@@ -2735,7 +2764,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="38"/>
+      <c r="A6" s="45"/>
       <c r="B6" s="9" t="s">
         <v>19</v>
       </c>
@@ -2744,7 +2773,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
+      <c r="A7" s="45"/>
       <c r="B7" s="9" t="s">
         <v>18</v>
       </c>
@@ -2753,7 +2782,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="38"/>
+      <c r="A8" s="45"/>
       <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
@@ -2762,7 +2791,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="38"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="9" t="s">
         <v>7</v>
       </c>
@@ -2771,7 +2800,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
+      <c r="A10" s="45"/>
       <c r="B10" s="9" t="s">
         <v>11</v>
       </c>
@@ -2781,7 +2810,7 @@
       <c r="D10" s="14"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="38"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="6" t="s">
         <v>12</v>
       </c>
@@ -2791,7 +2820,7 @@
       <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
+      <c r="A12" s="45"/>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
@@ -2804,7 +2833,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="38"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
@@ -2815,7 +2844,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
@@ -2828,7 +2857,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="38"/>
+      <c r="A15" s="45"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
@@ -2880,7 +2909,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="41" t="s">
         <v>307</v>
       </c>
       <c r="B2" s="36" t="s">
@@ -2888,7 +2917,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="42" t="s">
         <v>309</v>
       </c>
       <c r="B3" s="37" t="s">
@@ -2896,7 +2925,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="42" t="s">
         <v>310</v>
       </c>
       <c r="B4" s="37" t="s">
@@ -2904,10 +2933,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="38" t="s">
         <v>311</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="39" t="s">
         <v>312</v>
       </c>
       <c r="C5" t="s">
@@ -2915,15 +2944,15 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="42" t="s">
         <v>313</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="40" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="42" t="s">
         <v>314</v>
       </c>
       <c r="B7" s="37" t="s">
@@ -2931,7 +2960,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="42" t="s">
         <v>315</v>
       </c>
       <c r="B8" s="37" t="s">
@@ -2939,10 +2968,10 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="38" t="s">
         <v>316</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="39" t="s">
         <v>312</v>
       </c>
       <c r="C9" t="s">
@@ -2950,48 +2979,48 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="43" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="43" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="43" t="s">
         <v>322</v>
       </c>
       <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D14" s="44" t="s">
+      <c r="D14" s="43" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="43" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D16" s="44" t="s">
+      <c r="D16" s="43" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D17" s="44" t="s">
+      <c r="D17" s="43" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D18" s="44" t="s">
+      <c r="D18" s="43" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="19" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D19" s="44" t="s">
+      <c r="D19" s="43" t="s">
         <v>328</v>
       </c>
     </row>
@@ -3005,8 +3034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A123" sqref="A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3765,7 +3794,7 @@
       </c>
     </row>
     <row r="131" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+      <c r="A131" s="16" t="s">
         <v>320</v>
       </c>
       <c r="D131" s="31" t="s">
@@ -3894,68 +3923,101 @@
         <v>294</v>
       </c>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D145" s="45" t="s">
+    <row r="145" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D145" s="44" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D146" s="45" t="s">
+      <c r="E145" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="146" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D146" s="44" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E146" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="147" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D147" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D148" s="45" t="s">
+      <c r="E147" s="44" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="148" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D148" s="44" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E148" s="44" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="149" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D149" s="17" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D150" s="45" t="s">
+      <c r="E149" s="44" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="150" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D150" s="44" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E150" s="44" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="151" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D151" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="E151" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="152" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D152" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D153" s="45" t="s">
+      <c r="E152" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="153" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D153" s="44" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D154" s="45" t="s">
+      <c r="E153" s="17" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="154" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D154" s="44" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D155" s="45" t="s">
+      <c r="E154" s="17" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="155" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D155" s="44" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D156" s="45" t="s">
+      <c r="E155" s="17" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="156" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D156" s="44" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="157" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D157" s="45" t="s">
+    <row r="157" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D157" s="44" t="s">
         <v>301</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update of reference M20V functionality and list generation.
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="378">
   <si>
     <t>hashId</t>
   </si>
@@ -1065,17 +1065,145 @@
   <si>
     <t>MAAS00221</t>
   </si>
+  <si>
+    <t>Pobranie wszystkich rekordów danej referencji z jej wolumenem</t>
+  </si>
+  <si>
+    <t>SELECT m20vref, total FROM `toolshighrunner` WHERE m20vref='M20V00685'</t>
+  </si>
+  <si>
+    <t>Pobranie unikalnych wszystkich referencji M20V*</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT m20vref FROM `toolshighrunner` ORDER BY m20vref</t>
+  </si>
+  <si>
+    <t>Pobieram wszystkie referencje FA/BA dla każdej referencji unikalnej</t>
+  </si>
+  <si>
+    <t>Pobieram wszystkie unikalne referencje, razem z flow</t>
+  </si>
+  <si>
+    <t>Pobieram wolumen dla każdej unikalnej referencji</t>
+  </si>
+  <si>
+    <t>Pobieram wszystkie narzędzia dla każdej unikalnej referencji</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT m20vref, m20v FROM `toolshighrunner` ORDER BY m20vref</t>
+  </si>
+  <si>
+    <t>Pobranie unikalnych wszystkich referencji M20V* razem z flow</t>
+  </si>
+  <si>
+    <t>Pobranie sumarycznego wolumenu dla danej referencji</t>
+  </si>
+  <si>
+    <t>SELECT m20vref, SUM(total) FROM toolshighrunner WHERE m20vref='M20V00685'</t>
+  </si>
+  <si>
+    <t>Określam typ wolumenu dla każdej unikalnej referencji - skopiowanie funkcji getToolingRunnerTypeWithVolume</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT massref FROM `toolshighrunner` WHERE m20vref='M20V00685'</t>
+  </si>
+  <si>
+    <t>Pobranie unikalnej listy referencji MASS dla danej referencji M20V</t>
+  </si>
+  <si>
+    <t>Pobranie listy narzędzi zawierających daną raferencję M20v</t>
+  </si>
+  <si>
+    <t>SELECT toolstoolinglist.hashId FROM toolstoolinglist, toolsm20vconnection, toolsm20vref WHERE toolsm20vref.name='M20V00685' AND toolstoolinglist.hashId=toolsm20vconnection.hashId AND toolsm20vconnection.m20vId=toolsm20vref.m20vId</t>
+  </si>
+  <si>
+    <t>Pobranie listy numerów Hash, numeru narzędzia i id statusu zawierajacych daną referencję</t>
+  </si>
+  <si>
+    <t>SELECT toolstoolinglist.hashId, toolstoolinglist.toolingNo, toolstoolinglist.status FROM toolstoolinglist, toolsm20vconnection, toolsm20vref WHERE toolsm20vref.name='M20V00685' AND toolstoolinglist.hashId=toolsm20vconnection.hashId AND toolsm20vconnection.m20vId=toolsm20vref.m20vId</t>
+  </si>
+  <si>
+    <t>SELECT toolstoolinglist.hashId, toolstoolinglist.toolingNo, toolsstatus.name FROM toolstoolinglist, toolsm20vconnection, toolsm20vref, toolsstatus WHERE toolsm20vref.name='M20V00685' AND toolstoolinglist.hashId=toolsm20vconnection.hashId AND toolsm20vconnection.m20vId=toolsm20vref.m20vId AND toolsstatus.id=toolstoolinglist.status</t>
+  </si>
+  <si>
+    <t>SELECT toolsprocess.name, toolstoolinglist.hashId, toolstoolinglist.toolingNo, toolsstatus.name FROM toolstoolinglist, toolsm20vconnection, toolsm20vref, toolsstatus, toolsprocess WHERE toolsm20vref.name='M20V00685' AND toolstoolinglist.hashId=toolsm20vconnection.hashId AND toolsm20vconnection.m20vId=toolsm20vref.m20vId AND toolsstatus.id=toolstoolinglist.status AND toolstoolinglist.processId=toolsprocess.processId</t>
+  </si>
+  <si>
+    <t>Pobranie numeru hash, numeru narzedzia i statusu narzedzia dla danej referencji m20v</t>
+  </si>
+  <si>
+    <t>Pobranie typu procesu, numeru hash, nr narzedzia i statusu każdego narzędzia dla danej referencji m20v</t>
+  </si>
+  <si>
+    <t>Pobranie typu procesu, numeru hash, nr narzedzia i statusu każdego narzędzia dla danej referencji m20v z innymi nazwami kolumn</t>
+  </si>
+  <si>
+    <t>SELECT toolsprocess.name as processType, toolstoolinglist.hashId as hashNo, toolstoolinglist.toolingNo, toolsstatus.name as toolingStatus FROM toolstoolinglist, toolsm20vconnection, toolsm20vref, toolsstatus, toolsprocess WHERE toolsm20vref.name='M20V00685' AND toolstoolinglist.hashId=toolsm20vconnection.hashId AND toolsm20vconnection.m20vId=toolsm20vref.m20vId AND toolsstatus.id=toolstoolinglist.status AND toolstoolinglist.processId=toolsprocess.processId</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT m20vref as refa, (SELECT SUM(total) FROM toolshighrunner WHERE m20vref=refa</t>
+  </si>
+  <si>
+    <t>) as wolumen FROM toolshighrunner ORDER by wolumen DESC</t>
+  </si>
+  <si>
+    <t>) as wolumen, m20v FROM toolshighrunner ORDER by wolumen DESC</t>
+  </si>
+  <si>
+    <t>) as wolumen, m20v, (SELECT COUNT(toolstoolinglist.hashId) FROM toolstoolinglist, toolsm20vconnection, toolsm20vref WHERE toolsm20vref.name=refa AND toolstoolinglist.hashId=toolsm20vconnection.hashId AND toolsm20vconnection.m20vId=toolsm20vref.m20vId</t>
+  </si>
+  <si>
+    <t>) as tool FROM toolshighrunner ORDER by wolumen DESC</t>
+  </si>
+  <si>
+    <t>Pobranie referencji FA, sumy wolumenu, flow, liczbe narzedzi za pomoca jednego zapytania</t>
+  </si>
+  <si>
+    <t>) as tool, (SELECT DISTINCT COUNT(massref) FROM `toolshighrunner` WHERE m20vref=refa</t>
+  </si>
+  <si>
+    <t>) as mass FROM toolshighrunner ORDER by wolumen DESC</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT m20vref as refa, (SELECT SUM(total) FROM toolshighrunner WHERE m20vref=refa ) as wolumen, m20v, (SELECT COUNT(toolstoolinglist.hashId) FROM toolstoolinglist, toolsm20vconnection, toolsm20vref WHERE toolsm20vref.name=refa AND toolstoolinglist.hashId=toolsm20vconnection.hashId AND toolsm20vconnection.m20vId=toolsm20vref.m20vId ) as tool, (SELECT COUNT(DISTINCT massref) FROM `toolshighrunner` WHERE m20vref=refa ) as mass FROM toolshighrunner ORDER by wolumen DESC</t>
+  </si>
+  <si>
+    <t>koniec</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT m20vref as refa, (SELECT SUM(total) FROM toolshighrunner WHERE m20vref=refa ) as wolumen, m20v, (SELECT COUNT(toolstoolinglist.hashId) FROM toolstoolinglist, toolsm20vconnection, toolsm20vref WHERE toolsm20vref.name=refa AND toolstoolinglist.hashId=toolsm20vconnection.hashId AND toolsm20vconnection.m20vId=toolsm20vref.m20vId ) as tool, (SELECT COUNT(DISTINCT massref) FROM `toolshighrunner` WHERE m20vref=refa ) as mass FROM toolshighrunner ORDER by wolumen DESC LIMIT 0, 15</t>
+  </si>
+  <si>
+    <t>Pobranie wszystkich danych do glownej listy - tylko 15 pozycji (4,5 sek)</t>
+  </si>
+  <si>
+    <t>Pobranie wszystkich danych do glownej listy  (4,6 sek)</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT massref as refa, (SELECT SUM(total) FROM toolshighrunner WHERE massref=refa ) as wolumen, mass, (SELECT COUNT(toolstoolinglist.hashId) FROM toolstoolinglist, toolsmassconnection, toolsmassref WHERE toolsmassref.name=refa AND toolstoolinglist.hashId=toolsmassconnection.hashId AND toolsmassconnection.massId=toolsmassref.massId ) as tool, (SELECT COUNT(DISTINCT m20vref) FROM `toolshighrunner` WHERE massref=refa ) as final FROM toolshighrunner ORDER by wolumen DESC</t>
+  </si>
+  <si>
+    <t>Pobranie wszystkich danych MASS do głównej listy (4,6 sek)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1390,10 +1518,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1410,24 +1538,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1436,35 +1564,37 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -2158,7 +2288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -2728,7 +2858,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="47" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -2737,7 +2867,7 @@
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
+      <c r="A3" s="47"/>
       <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
@@ -2746,7 +2876,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
@@ -2755,7 +2885,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
@@ -2764,7 +2894,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="9" t="s">
         <v>19</v>
       </c>
@@ -2773,7 +2903,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="9" t="s">
         <v>18</v>
       </c>
@@ -2782,7 +2912,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
@@ -2791,7 +2921,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="45"/>
+      <c r="A9" s="47"/>
       <c r="B9" s="9" t="s">
         <v>7</v>
       </c>
@@ -2800,7 +2930,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="9" t="s">
         <v>11</v>
       </c>
@@ -2810,7 +2940,7 @@
       <c r="D10" s="14"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="45"/>
+      <c r="A11" s="47"/>
       <c r="B11" s="6" t="s">
         <v>12</v>
       </c>
@@ -2820,7 +2950,7 @@
       <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
+      <c r="A12" s="47"/>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
@@ -2833,7 +2963,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="45"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
@@ -2844,7 +2974,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
@@ -2857,7 +2987,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="45"/>
+      <c r="A15" s="47"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7" t="s">
@@ -3034,8 +3164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="A123" sqref="A123"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A122" sqref="A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4032,10 +4162,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F100"/>
+  <dimension ref="A1:AZ153"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="A154" sqref="A154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4652,25 +4782,335 @@
         <v>196</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>204</v>
       </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="45">
+        <v>42841</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="16" t="s">
+        <v>346</v>
+      </c>
+      <c r="B108" s="16"/>
+      <c r="C108" s="16"/>
+      <c r="D108" s="16"/>
+      <c r="E108" s="16"/>
+      <c r="F108" s="16"/>
+      <c r="G108" s="16"/>
+      <c r="H108" s="16"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" s="46" t="s">
+        <v>349</v>
+      </c>
+      <c r="B110" s="16"/>
+      <c r="C110" s="16"/>
+      <c r="D110" s="16"/>
+      <c r="E110" s="16"/>
+      <c r="F110" s="16"/>
+      <c r="G110" s="16"/>
+      <c r="H110" s="16"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" s="16" t="s">
+        <v>351</v>
+      </c>
+      <c r="B112" s="16"/>
+      <c r="C112" s="16"/>
+      <c r="D112" s="16"/>
+      <c r="E112" s="16"/>
+      <c r="F112" s="16"/>
+      <c r="G112" s="16"/>
+      <c r="H112" s="16"/>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A114" s="16" t="s">
+        <v>354</v>
+      </c>
+      <c r="B114" s="16"/>
+      <c r="C114" s="16"/>
+      <c r="D114" s="16"/>
+      <c r="E114" s="16"/>
+      <c r="F114" s="16"/>
+      <c r="G114" s="16"/>
+      <c r="H114" s="16"/>
+      <c r="I114" s="16"/>
+      <c r="J114" s="16"/>
+      <c r="K114" s="16"/>
+      <c r="L114" s="16"/>
+      <c r="M114" s="16"/>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A122" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="B122" s="16"/>
+      <c r="C122" s="16"/>
+      <c r="D122" s="16"/>
+      <c r="E122" s="16"/>
+      <c r="F122" s="16"/>
+      <c r="G122" s="16"/>
+      <c r="H122" s="16"/>
+      <c r="I122" s="16"/>
+      <c r="J122" s="16"/>
+      <c r="K122" s="16"/>
+      <c r="L122" s="16"/>
+      <c r="M122" s="16"/>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="145" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="147" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>371</v>
+      </c>
+      <c r="AZ147" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="148" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="149" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A149" s="16" t="s">
+        <v>371</v>
+      </c>
+      <c r="B149" s="16"/>
+      <c r="C149" s="16"/>
+      <c r="D149" s="16"/>
+      <c r="E149" s="16"/>
+      <c r="F149" s="16"/>
+      <c r="G149" s="16"/>
+      <c r="H149" s="16"/>
+      <c r="I149" s="16"/>
+      <c r="J149" s="16"/>
+      <c r="K149" s="16"/>
+      <c r="L149" s="16"/>
+      <c r="M149" s="16"/>
+      <c r="N149" s="16"/>
+      <c r="O149" s="16"/>
+      <c r="P149" s="16"/>
+      <c r="Q149" s="16"/>
+      <c r="R149" s="16"/>
+      <c r="AZ149" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="150" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="151" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="152" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="153" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A153" s="16" t="s">
+        <v>376</v>
+      </c>
+      <c r="B153" s="16"/>
+      <c r="C153" s="16"/>
+      <c r="D153" s="16"/>
+      <c r="E153" s="16"/>
+      <c r="F153" s="16"/>
+      <c r="G153" s="16"/>
+      <c r="H153" s="16"/>
+      <c r="I153" s="16"/>
+      <c r="J153" s="16"/>
+      <c r="K153" s="16"/>
+      <c r="L153" s="16"/>
+      <c r="M153" s="16"/>
+      <c r="N153" s="16"/>
+      <c r="O153" s="16"/>
+      <c r="P153" s="16"/>
+      <c r="Q153" s="16"/>
+      <c r="R153" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>